<commit_message>
fix Database dan Panduan
</commit_message>
<xml_diff>
--- a/Panduan Import Export.xlsx
+++ b/Panduan Import Export.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ALDO\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Kuliah\KP 2020\Project\admin-data-GKJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2BDEFE-DBFC-45F5-9552-3AC9664C4C30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21A709F-38E6-403F-9D2F-035A6DA997DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{049EC426-CB20-4A5D-99CF-B8058632C40B}"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{049EC426-CB20-4A5D-99CF-B8058632C40B}"/>
   </bookViews>
   <sheets>
     <sheet name="Panduan" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>no</t>
   </si>
@@ -313,6 +313,30 @@
   </si>
   <si>
     <t>0274-585687</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Belum Sekolah</t>
+  </si>
+  <si>
+    <t>Wilayah Selatan</t>
+  </si>
+  <si>
+    <t>Wilayah Timur B</t>
+  </si>
+  <si>
+    <t>Wilayah Timur A</t>
+  </si>
+  <si>
+    <t>Wilayah Barat</t>
+  </si>
+  <si>
+    <t>Maksimal 800 data dalam sekali import</t>
   </si>
 </sst>
 </file>
@@ -466,40 +490,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -815,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59ACD577-00B4-4622-BAD9-EADDF00AD6F0}">
-  <dimension ref="B2:V17"/>
+  <dimension ref="B2:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,7 +855,7 @@
     <col min="6" max="6" width="16" style="2" customWidth="1"/>
     <col min="7" max="7" width="3.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="3.5703125" style="2" customWidth="1"/>
     <col min="11" max="11" width="8.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="13.7109375" style="2" customWidth="1"/>
@@ -840,7 +864,7 @@
     <col min="15" max="15" width="12" style="2" customWidth="1"/>
     <col min="16" max="16" width="3.5703125" style="2" customWidth="1"/>
     <col min="17" max="17" width="8.28515625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13" style="2" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="2" customWidth="1"/>
     <col min="19" max="19" width="3.5703125" style="2" customWidth="1"/>
     <col min="20" max="20" width="8.28515625" style="2" customWidth="1"/>
     <col min="21" max="21" width="17.140625" style="2" customWidth="1"/>
@@ -848,34 +872,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="E2" s="11" t="s">
+      <c r="C2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="H2" s="10" t="s">
+      <c r="F2" s="21"/>
+      <c r="H2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="I2" s="20"/>
+      <c r="K2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="N2" s="10" t="s">
+      <c r="L2" s="20"/>
+      <c r="N2" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="Q2" s="10" t="s">
+      <c r="O2" s="20"/>
+      <c r="Q2" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="10"/>
-      <c r="T2" s="10" t="s">
+      <c r="R2" s="20"/>
+      <c r="T2" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="10"/>
+      <c r="U2" s="20"/>
     </row>
     <row r="3" spans="2:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1189,6 +1213,12 @@
       <c r="I14" s="9">
         <v>11</v>
       </c>
+      <c r="Q14" s="6">
+        <v>11</v>
+      </c>
+      <c r="R14" s="9" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H15" s="6">
@@ -1197,6 +1227,12 @@
       <c r="I15" s="9">
         <v>12</v>
       </c>
+      <c r="Q15" s="6">
+        <v>12</v>
+      </c>
+      <c r="R15" s="9" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="16" spans="2:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H16" s="6">
@@ -1205,6 +1241,12 @@
       <c r="I16" s="9">
         <v>13</v>
       </c>
+      <c r="Q16" s="6">
+        <v>13</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="17" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H17" s="6">
@@ -1212,6 +1254,38 @@
       </c>
       <c r="I17" s="9">
         <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="6">
+        <v>15</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="6">
+        <v>16</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="6">
+        <v>17</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H21" s="6">
+        <v>18</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1225,6 +1299,7 @@
     <mergeCell ref="Q2:R2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1232,8 +1307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9999C889-6C46-4EE3-B6D4-8AC43BD30BAE}">
   <dimension ref="B2:Z10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,214 +1341,222 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:26" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
     </row>
     <row r="4" spans="2:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="2:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" spans="2:26" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>3</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="8" spans="2:26" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="L9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="M9" s="16" t="s">
+      <c r="M9" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="N9" s="15" t="s">
+      <c r="N9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="16" t="s">
+      <c r="O9" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="Q9" s="16" t="s">
+      <c r="Q9" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="R9" s="15" t="s">
+      <c r="R9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="S9" s="17" t="s">
+      <c r="S9" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="T9" s="16" t="s">
+      <c r="T9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="U9" s="16" t="s">
+      <c r="U9" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="V9" s="16" t="s">
+      <c r="V9" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="W9" s="15" t="s">
+      <c r="W9" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="X9" s="17" t="s">
+      <c r="X9" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="Y9" s="16" t="s">
+      <c r="Y9" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="Z9" s="18" t="s">
+      <c r="Z9" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="19">
+      <c r="B10" s="17">
         <v>2</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="17">
         <v>3</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="17">
         <v>1</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="18">
         <v>20566</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="17">
         <v>1</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="17">
         <v>4</v>
       </c>
-      <c r="K10" s="19" t="s">
+      <c r="K10" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="M10" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="N10" s="19">
+      <c r="N10" s="17">
         <v>4</v>
       </c>
-      <c r="O10" s="19" t="s">
+      <c r="O10" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="P10" s="19" t="s">
+      <c r="P10" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="Q10" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="R10" s="19">
+      <c r="R10" s="17">
         <v>2</v>
       </c>
-      <c r="S10" s="20">
+      <c r="S10" s="18">
         <v>36717</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="T10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="U10" s="19" t="s">
+      <c r="U10" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="V10" s="19" t="s">
+      <c r="V10" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="W10" s="19">
+      <c r="W10" s="17">
         <v>2</v>
       </c>
-      <c r="X10" s="20">
+      <c r="X10" s="18">
         <v>40588</v>
       </c>
-      <c r="Y10" s="19" t="s">
+      <c r="Y10" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="Z10" s="20">
+      <c r="Z10" s="18">
         <v>41364</v>
       </c>
     </row>

</xml_diff>